<commit_message>
Added getcaptain match funtions
</commit_message>
<xml_diff>
--- a/api keys.xlsx
+++ b/api keys.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t>Email Id</t>
   </si>
@@ -93,6 +95,39 @@
   </si>
   <si>
     <t>ankit email 1</t>
+  </si>
+  <si>
+    <t>ySAewUr5vLamX7LLdfzYD7jTWiJ2</t>
+  </si>
+  <si>
+    <t>ilzY7ckWVyQfjtULC8uiU2ciSW93</t>
+  </si>
+  <si>
+    <t>fvxbB9BLVNfxatmOaiseF7Jzz6B2</t>
+  </si>
+  <si>
+    <t>Klr0NkJuG3YpZ1KburbMBNpfO1q1</t>
+  </si>
+  <si>
+    <t>minues</t>
+  </si>
+  <si>
+    <t>Matches</t>
+  </si>
+  <si>
+    <t>No Kyes</t>
+  </si>
+  <si>
+    <t>Hits for match detials</t>
+  </si>
+  <si>
+    <t>Tottal hits for stats details</t>
+  </si>
+  <si>
+    <t>Total Hits</t>
+  </si>
+  <si>
+    <t>Hits per keys</t>
   </si>
 </sst>
 </file>
@@ -440,7 +475,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +581,9 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -555,7 +592,9 @@
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -564,7 +603,9 @@
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -573,7 +614,9 @@
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -614,4 +657,258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1">
+        <f>60/A1*4*A2</f>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <f>SUM(F1:F2)</f>
+        <v>968</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5">
+        <f>F3/A3</f>
+        <v>32.266666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>